<commit_message>
data dictionary tagged with features to keep
</commit_message>
<xml_diff>
--- a/data/LCDataDictionary.xlsx
+++ b/data/LCDataDictionary.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rjoshi/Documents/LendingClub/Quarterly_Loan_Stats/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NB24125\Documents\loan-data-analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22620" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="38400" windowHeight="22620"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="RejectStats" sheetId="7" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$C$89</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$129</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="384">
   <si>
     <t>id</t>
   </si>
@@ -1197,11 +1197,14 @@
   <si>
     <t>The method by which the borrower receives their loan. Possible values are: CASH, DIRECT_PAY</t>
   </si>
+  <si>
+    <t>KeepIt</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1571,7 +1574,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1723,6 +1726,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1818,7 +1832,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1856,100 +1870,101 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="92">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="67" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="66" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Hipervínculo" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="64" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="66" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="68" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="70" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="65" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="67" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="69" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="71" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2251,25 +2266,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145:B145"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="122.140625" customWidth="1"/>
+    <col min="3" max="3" width="118.85546875" style="6" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>99</v>
       </c>
@@ -2277,7 +2292,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>291</v>
       </c>
@@ -2286,7 +2301,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>295</v>
       </c>
@@ -2295,7 +2310,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
@@ -2304,7 +2319,7 @@
       </c>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>285</v>
       </c>
@@ -2313,7 +2328,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -2322,7 +2337,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
@@ -2331,7 +2346,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>252</v>
       </c>
@@ -2340,7 +2355,7 @@
       </c>
       <c r="C8" s="5"/>
     </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>114</v>
       </c>
@@ -2349,7 +2364,7 @@
       </c>
       <c r="C9" s="5"/>
     </row>
-    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>296</v>
       </c>
@@ -2358,7 +2373,7 @@
       </c>
       <c r="C10" s="5"/>
     </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>297</v>
       </c>
@@ -2367,7 +2382,7 @@
       </c>
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>105</v>
       </c>
@@ -2376,7 +2391,7 @@
       </c>
       <c r="C12" s="5"/>
     </row>
-    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>226</v>
       </c>
@@ -2385,7 +2400,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>106</v>
       </c>
@@ -2394,7 +2409,7 @@
       </c>
       <c r="C14" s="5"/>
     </row>
-    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -2403,7 +2418,7 @@
       </c>
       <c r="C15" s="24"/>
     </row>
-    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>298</v>
       </c>
@@ -2412,7 +2427,7 @@
       </c>
       <c r="C16" s="24"/>
     </row>
-    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -2421,7 +2436,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="4" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>21</v>
       </c>
@@ -2430,7 +2445,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>255</v>
       </c>
@@ -2439,7 +2454,7 @@
       </c>
       <c r="C19" s="5"/>
     </row>
-    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
@@ -2448,7 +2463,7 @@
       </c>
       <c r="C20" s="5"/>
     </row>
-    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -2457,7 +2472,7 @@
       </c>
       <c r="C21" s="5"/>
     </row>
-    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>166</v>
       </c>
@@ -2466,7 +2481,7 @@
       </c>
       <c r="C22" s="5"/>
     </row>
-    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -2475,7 +2490,7 @@
       </c>
       <c r="C23" s="5"/>
     </row>
-    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -2484,7 +2499,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>3</v>
       </c>
@@ -2493,7 +2508,7 @@
       </c>
       <c r="C25" s="5"/>
     </row>
-    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -2502,7 +2517,7 @@
       </c>
       <c r="C26" s="5"/>
     </row>
-    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -2511,7 +2526,7 @@
       </c>
       <c r="C27" s="5"/>
     </row>
-    <row r="28" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>11</v>
       </c>
@@ -2520,7 +2535,7 @@
       </c>
       <c r="C28" s="5"/>
     </row>
-    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -2529,7 +2544,7 @@
       </c>
       <c r="C29" s="24"/>
     </row>
-    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>277</v>
       </c>
@@ -2538,7 +2553,7 @@
       </c>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -2547,7 +2562,7 @@
       </c>
       <c r="C31" s="5"/>
     </row>
-    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>287</v>
       </c>
@@ -2556,7 +2571,7 @@
       </c>
       <c r="C32" s="5"/>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>289</v>
       </c>
@@ -2565,7 +2580,7 @@
       </c>
       <c r="C33" s="5"/>
     </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>26</v>
       </c>
@@ -2574,7 +2589,7 @@
       </c>
       <c r="C34" s="5"/>
     </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>7</v>
       </c>
@@ -2583,7 +2598,7 @@
       </c>
       <c r="C35" s="5"/>
     </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>6</v>
       </c>
@@ -2592,7 +2607,7 @@
       </c>
       <c r="C36" s="5"/>
     </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>13</v>
       </c>
@@ -2603,7 +2618,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -2612,7 +2627,7 @@
       </c>
       <c r="C38" s="5"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -2621,7 +2636,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -2630,7 +2645,7 @@
       </c>
       <c r="D40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -2639,7 +2654,7 @@
       </c>
       <c r="D41" s="4"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -2648,7 +2663,7 @@
       </c>
       <c r="D42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>2</v>
       </c>
@@ -2657,7 +2672,7 @@
       </c>
       <c r="D43" s="4"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2681,7 @@
       </c>
       <c r="D44" s="4"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>283</v>
       </c>
@@ -2675,7 +2690,7 @@
       </c>
       <c r="D45" s="4"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -2687,7 +2702,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>299</v>
       </c>
@@ -2699,7 +2714,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>124</v>
       </c>
@@ -2711,7 +2726,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>125</v>
       </c>
@@ -2720,7 +2735,7 @@
       </c>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>111</v>
       </c>
@@ -2729,7 +2744,7 @@
       </c>
       <c r="D50" s="4"/>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>300</v>
       </c>
@@ -2738,7 +2753,7 @@
       </c>
       <c r="D51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>27</v>
       </c>
@@ -2747,7 +2762,7 @@
       </c>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>108</v>
       </c>
@@ -2756,7 +2771,7 @@
       </c>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -2765,7 +2780,7 @@
       </c>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>273</v>
       </c>
@@ -2774,7 +2789,7 @@
       </c>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>301</v>
       </c>
@@ -2783,7 +2798,7 @@
       </c>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>302</v>
       </c>
@@ -2792,7 +2807,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>304</v>
       </c>
@@ -2801,7 +2816,7 @@
       </c>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>305</v>
       </c>
@@ -2810,7 +2825,7 @@
       </c>
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -2819,7 +2834,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>104</v>
       </c>
@@ -2828,7 +2843,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>116</v>
       </c>
@@ -2836,7 +2851,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>123</v>
       </c>
@@ -2844,7 +2859,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>117</v>
       </c>
@@ -2852,7 +2867,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>115</v>
       </c>
@@ -2860,7 +2875,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>122</v>
       </c>
@@ -2868,7 +2883,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>127</v>
       </c>
@@ -2876,7 +2891,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>102</v>
       </c>
@@ -2884,7 +2899,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>126</v>
       </c>
@@ -2892,7 +2907,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>109</v>
       </c>
@@ -2900,7 +2915,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>121</v>
       </c>
@@ -2908,7 +2923,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>120</v>
       </c>
@@ -2916,7 +2931,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>119</v>
       </c>
@@ -2926,7 +2941,7 @@
       <c r="C73"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>110</v>
       </c>
@@ -2934,7 +2949,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>29</v>
       </c>
@@ -2942,7 +2957,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>266</v>
       </c>
@@ -2950,7 +2965,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>269</v>
       </c>
@@ -2958,7 +2973,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>271</v>
       </c>
@@ -2966,7 +2981,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>335</v>
       </c>
@@ -2974,7 +2989,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>279</v>
       </c>
@@ -2982,7 +2997,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>281</v>
       </c>
@@ -2990,7 +3005,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -2998,7 +3013,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -3006,7 +3021,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>118</v>
       </c>
@@ -3014,7 +3029,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>306</v>
       </c>
@@ -3022,7 +3037,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>129</v>
       </c>
@@ -3030,7 +3045,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>30</v>
       </c>
@@ -3038,7 +3053,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>103</v>
       </c>
@@ -3046,7 +3061,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>18</v>
       </c>
@@ -3054,7 +3069,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>15</v>
       </c>
@@ -3062,7 +3077,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>225</v>
       </c>
@@ -3070,7 +3085,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>31</v>
       </c>
@@ -3078,7 +3093,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>32</v>
       </c>
@@ -3086,7 +3101,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>9</v>
       </c>
@@ -3094,7 +3109,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>107</v>
       </c>
@@ -3102,7 +3117,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>5</v>
       </c>
@@ -3110,7 +3125,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>19</v>
       </c>
@@ -3118,7 +3133,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>128</v>
       </c>
@@ -3126,7 +3141,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>113</v>
       </c>
@@ -3134,7 +3149,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>112</v>
       </c>
@@ -3142,7 +3157,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>33</v>
       </c>
@@ -3150,7 +3165,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>307</v>
       </c>
@@ -3158,7 +3173,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>275</v>
       </c>
@@ -3166,7 +3181,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>308</v>
       </c>
@@ -3174,7 +3189,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>293</v>
       </c>
@@ -3182,7 +3197,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="9" t="s">
         <v>100</v>
       </c>
@@ -3190,7 +3205,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -3198,7 +3213,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -3206,7 +3221,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -3214,7 +3229,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -3222,7 +3237,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -3230,7 +3245,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" s="9" t="s">
         <v>217</v>
       </c>
@@ -3238,7 +3253,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -3246,7 +3261,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>294</v>
       </c>
@@ -3254,7 +3269,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>257</v>
       </c>
@@ -3262,7 +3277,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>247</v>
       </c>
@@ -3270,7 +3285,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
         <v>310</v>
       </c>
@@ -3278,7 +3293,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
         <v>312</v>
       </c>
@@ -3286,7 +3301,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
         <v>314</v>
       </c>
@@ -3294,7 +3309,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
         <v>316</v>
       </c>
@@ -3302,7 +3317,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="18" t="s">
         <v>318</v>
       </c>
@@ -3310,7 +3325,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="18" t="s">
         <v>320</v>
       </c>
@@ -3318,7 +3333,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="18" t="s">
         <v>322</v>
       </c>
@@ -3326,7 +3341,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="18" t="s">
         <v>324</v>
       </c>
@@ -3334,7 +3349,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="18" t="s">
         <v>336</v>
       </c>
@@ -3342,7 +3357,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="18" t="s">
         <v>327</v>
       </c>
@@ -3350,7 +3365,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="18" t="s">
         <v>329</v>
       </c>
@@ -3358,7 +3373,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="18" t="s">
         <v>331</v>
       </c>
@@ -3366,7 +3381,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="18" t="s">
         <v>333</v>
       </c>
@@ -3374,7 +3389,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="9" t="s">
         <v>347</v>
       </c>
@@ -3382,7 +3397,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="9" t="s">
         <v>348</v>
       </c>
@@ -3390,7 +3405,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="9" t="s">
         <v>349</v>
       </c>
@@ -3398,7 +3413,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="9" t="s">
         <v>350</v>
       </c>
@@ -3406,7 +3421,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="9" t="s">
         <v>351</v>
       </c>
@@ -3414,7 +3429,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="9" t="s">
         <v>352</v>
       </c>
@@ -3422,7 +3437,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="9" t="s">
         <v>353</v>
       </c>
@@ -3430,7 +3445,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="9" t="s">
         <v>354</v>
       </c>
@@ -3438,7 +3453,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="9" t="s">
         <v>355</v>
       </c>
@@ -3446,7 +3461,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="9" t="s">
         <v>356</v>
       </c>
@@ -3454,7 +3469,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="9" t="s">
         <v>357</v>
       </c>
@@ -3462,7 +3477,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="9" t="s">
         <v>358</v>
       </c>
@@ -3470,7 +3485,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="9" t="s">
         <v>359</v>
       </c>
@@ -3478,7 +3493,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="9" t="s">
         <v>360</v>
       </c>
@@ -3486,7 +3501,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="9" t="s">
         <v>361</v>
       </c>
@@ -3494,7 +3509,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="9" t="s">
         <v>362</v>
       </c>
@@ -3502,7 +3517,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="9" t="s">
         <v>345</v>
       </c>
@@ -3510,7 +3525,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="9" t="s">
         <v>346</v>
       </c>
@@ -3518,7 +3533,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="9" t="s">
         <v>363</v>
       </c>
@@ -3526,7 +3541,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="s">
         <v>340</v>
       </c>
@@ -3534,7 +3549,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="s">
         <v>364</v>
       </c>
@@ -3542,7 +3557,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
         <v>365</v>
       </c>
@@ -3550,7 +3565,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
         <v>366</v>
       </c>
@@ -3558,7 +3573,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B154" s="13" t="s">
         <v>168</v>
       </c>
@@ -3575,1180 +3590,1354 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F123"/>
+  <dimension ref="A1:G123"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B121" sqref="B121"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="187.28515625" customWidth="1"/>
+    <col min="7" max="7" width="235.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>219</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>383</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="9">
+        <v>0</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="9">
+        <v>0</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="9">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>190</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="23">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="D5" s="6"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="9">
+        <v>0</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>265</v>
       </c>
-      <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="D8"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>252</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="C10" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="9">
+        <v>0</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="9">
+        <v>0</v>
+      </c>
+      <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="D14" s="6"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>187</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="9">
+        <v>0</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B16" s="9">
+        <v>0</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="6"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="9">
+        <v>0</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="6"/>
+    </row>
+    <row r="19" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="25">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>242</v>
       </c>
-      <c r="D19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="7">
+        <v>0</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="9">
+        <v>0</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="6"/>
       <c r="F21" s="6"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="3">
+        <v>0</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>238</v>
       </c>
-      <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>167</v>
       </c>
-      <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="6"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="9">
+        <v>0</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="B25" s="9">
+        <v>0</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="D25" s="6"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="B26" s="9" t="s">
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="D26" s="6"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="6"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B27" s="9"/>
+      <c r="C27" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="6"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B28" s="9" t="s">
+      <c r="B28" s="9"/>
+      <c r="C28" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="D28" s="6"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>171</v>
       </c>
-      <c r="B29" s="9" t="s">
+      <c r="B29" s="9"/>
+      <c r="C29" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="6"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="9"/>
+      <c r="C30" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="D30" s="6"/>
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="6"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="9"/>
+      <c r="C31" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="6"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="9"/>
+      <c r="C32" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="6"/>
       <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="6"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="9"/>
+      <c r="C33" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="E33" s="6"/>
       <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="6"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B34" s="11" t="s">
+      <c r="B34" s="11"/>
+      <c r="C34" s="11" t="s">
         <v>181</v>
       </c>
-      <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="6"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
         <v>216</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="9"/>
+      <c r="C35" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D35" s="6"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="9" t="s">
         <v>288</v>
       </c>
-      <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B37" s="9"/>
+      <c r="C37" s="9" t="s">
         <v>290</v>
       </c>
-      <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="9"/>
+      <c r="C38" s="7" t="s">
         <v>262</v>
       </c>
-      <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="9"/>
+      <c r="C39" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="9"/>
+      <c r="C40" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="D40" s="6"/>
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="9"/>
+      <c r="C41" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="E41" s="6"/>
       <c r="F41" s="6"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="B42" s="9" t="s">
+      <c r="B42" s="9"/>
+      <c r="C42" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="E42" s="6"/>
       <c r="F42" s="6"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E43" s="6"/>
       <c r="F43" s="6"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="B44" s="9" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="E44" s="6"/>
       <c r="F44" s="6"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="9"/>
+      <c r="C45" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="6"/>
       <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="9"/>
+      <c r="C46" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="9"/>
+      <c r="C47" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E47" s="6"/>
       <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B48" s="9"/>
+      <c r="C48" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="E48" s="6"/>
       <c r="F48" s="6"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="9" t="s">
         <v>208</v>
       </c>
-      <c r="B49" s="9" t="s">
+      <c r="B49" s="9"/>
+      <c r="C49" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B50" s="9"/>
+      <c r="C50" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="E50" s="6"/>
       <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G50" s="6"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B51" s="9" t="s">
+      <c r="B51" s="9"/>
+      <c r="C51" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="E51" s="6"/>
       <c r="F51" s="6"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G51" s="6"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B52" s="9" t="s">
+      <c r="B52" s="9"/>
+      <c r="C52" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="E52" s="6"/>
       <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G52" s="6"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="9"/>
+      <c r="C53" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="F53" s="6"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G53" s="6"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
         <v>202</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="9"/>
+      <c r="C54" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F54" s="6"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G54" s="6"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="9"/>
+      <c r="C55" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="F55" s="6"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G55" s="6"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="9"/>
+      <c r="C56" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="F56" s="6"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G56" s="6"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="9"/>
+      <c r="C57" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="F57" s="6"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G57" s="6"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="9"/>
+      <c r="C58" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="F58" s="6"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G58" s="6"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="9"/>
+      <c r="C59" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F59" s="6"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G59" s="6"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="9"/>
+      <c r="C60" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="F60" s="6"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G60" s="6"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="9"/>
+      <c r="C61" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="F61" s="6"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G61" s="6"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="9"/>
+      <c r="C62" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F62" s="6"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G62" s="6"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="9"/>
+      <c r="C63" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="F63" s="6"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G63" s="6"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="9"/>
+      <c r="C64" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="F64" s="6"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G64" s="6"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="9"/>
+      <c r="C65" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="F65" s="6"/>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G65" s="6"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="9"/>
+      <c r="C66" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="F66" s="6"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G66" s="6"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B67" s="9" t="s">
+      <c r="B67" s="9"/>
+      <c r="C67" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F67" s="6"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G67" s="6"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B68" s="9" t="s">
+      <c r="B68" s="9"/>
+      <c r="C68" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="F68" s="6"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G68" s="6"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="B69" s="9" t="s">
+      <c r="B69" s="9"/>
+      <c r="C69" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="F69" s="6"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G69" s="6"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="B70" s="9" t="s">
+      <c r="B70" s="9"/>
+      <c r="C70" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="D70" s="6"/>
-      <c r="F70" s="6"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E70" s="6"/>
+      <c r="G70" s="6"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="B71" s="9" t="s">
+      <c r="B71" s="9"/>
+      <c r="C71" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="F71" s="6"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G71" s="6"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="B72" s="9" t="s">
+      <c r="B72" s="9"/>
+      <c r="C72" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="F72" s="6"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G72" s="6"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B73" s="9"/>
+      <c r="C73" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="D73" s="6"/>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E73" s="6"/>
+      <c r="G73" s="6"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B74" s="8" t="s">
+      <c r="B74" s="9"/>
+      <c r="C74" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="D74" s="6"/>
-      <c r="F74" s="6"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E74" s="6"/>
+      <c r="G74" s="6"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="B75" s="9" t="s">
+      <c r="B75" s="9"/>
+      <c r="C75" s="9" t="s">
         <v>270</v>
       </c>
-      <c r="D75" s="6"/>
-      <c r="F75" s="6"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E75" s="6"/>
+      <c r="G75" s="6"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="B76" s="9" t="s">
+      <c r="B76" s="9"/>
+      <c r="C76" s="9" t="s">
         <v>272</v>
       </c>
-      <c r="F76" s="6"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G76" s="6"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="9" t="s">
         <v>335</v>
       </c>
-      <c r="B77" s="9" t="s">
+      <c r="B77" s="9"/>
+      <c r="C77" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="F77" s="6"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G77" s="6"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B78" s="9"/>
+      <c r="C78" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="D78" s="6"/>
-      <c r="F78" s="6"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E78" s="6"/>
+      <c r="G78" s="6"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B79" s="9" t="s">
+      <c r="B79" s="9"/>
+      <c r="C79" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="D79" s="6"/>
-      <c r="F79" s="6"/>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E79" s="6"/>
+      <c r="G79" s="6"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B80" s="9" t="s">
+      <c r="B80" s="9"/>
+      <c r="C80" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="F80" s="6"/>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G80" s="6"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B81" s="9" t="s">
+      <c r="B81" s="9"/>
+      <c r="C81" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="D81" s="6"/>
-      <c r="F81" s="6"/>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E81" s="6"/>
+      <c r="G81" s="6"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B82" s="9" t="s">
+      <c r="B82" s="9"/>
+      <c r="C82" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="D82" s="6"/>
-      <c r="F82" s="6"/>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E82" s="6"/>
+      <c r="G82" s="6"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B83" s="9" t="s">
+      <c r="B83" s="9"/>
+      <c r="C83" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="F83" s="6"/>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G83" s="6"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="9"/>
+      <c r="C84" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="F84" s="6"/>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B85" s="9" t="s">
+      <c r="B85" s="9"/>
+      <c r="C85" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="F85" s="6"/>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G85" s="6"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="9" t="s">
         <v>189</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="9"/>
+      <c r="C86" s="9" t="s">
         <v>164</v>
       </c>
-      <c r="F86" s="6"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G86" s="6"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B87" s="9"/>
+      <c r="C87" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="F87" s="6"/>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G87" s="6"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="9"/>
+      <c r="C88" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F88" s="6"/>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G88" s="6"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="B89" s="9" t="s">
+      <c r="B89" s="9"/>
+      <c r="C89" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F89" s="6"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G89" s="6"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="B90" s="9"/>
+      <c r="C90" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="F90" s="6"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G90" s="6"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B91" s="9" t="s">
+      <c r="B91" s="9"/>
+      <c r="C91" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="D91" s="6"/>
-      <c r="F91" s="6"/>
-    </row>
-    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="E91" s="6"/>
+      <c r="G91" s="6"/>
+    </row>
+    <row r="92" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B92" s="9"/>
+      <c r="C92" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D92"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E92"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B93" s="9" t="s">
+      <c r="B93" s="9"/>
+      <c r="C93" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D93" s="6"/>
-      <c r="F93" s="6"/>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E93" s="6"/>
+      <c r="G93" s="6"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B94" s="9" t="s">
+      <c r="B94" s="9"/>
+      <c r="C94" s="9" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="B95" s="9"/>
+      <c r="C95" s="9" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B96" s="9"/>
+      <c r="C96" s="9" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="B97" s="9" t="s">
+      <c r="B97" s="9"/>
+      <c r="C97" s="9" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B98" s="9" t="s">
+      <c r="B98" s="9"/>
+      <c r="C98" s="9" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="9" t="s">
         <v>293</v>
       </c>
-      <c r="B99" s="9" t="s">
+      <c r="B99" s="9"/>
+      <c r="C99" s="9" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B100" s="9" t="s">
+      <c r="B100" s="9"/>
+      <c r="C100" s="9" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B101" s="9" t="s">
+      <c r="B101" s="9"/>
+      <c r="C101" s="9" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="B102" s="9" t="s">
+      <c r="B102" s="9"/>
+      <c r="C102" s="9" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B103" s="9" t="s">
+      <c r="B103" s="9"/>
+      <c r="C103" s="9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="B104" s="9" t="s">
+      <c r="B104" s="9"/>
+      <c r="C104" s="9" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B105" s="9"/>
+      <c r="C105" s="9" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="B106" s="7" t="s">
+      <c r="B106" s="7"/>
+      <c r="C106" s="7" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="22" t="s">
         <v>247</v>
       </c>
-      <c r="B107" s="22" t="s">
+      <c r="B107" s="22"/>
+      <c r="C107" s="22" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="18" t="s">
         <v>310</v>
       </c>
-      <c r="B108" s="18" t="s">
+      <c r="B108" s="18"/>
+      <c r="C108" s="18" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="18" t="s">
         <v>312</v>
       </c>
-      <c r="B109" s="18" t="s">
+      <c r="B109" s="18"/>
+      <c r="C109" s="18" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="18" t="s">
         <v>314</v>
       </c>
-      <c r="B110" s="18" t="s">
+      <c r="B110" s="18"/>
+      <c r="C110" s="18" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="18" t="s">
         <v>316</v>
       </c>
-      <c r="B111" s="18" t="s">
+      <c r="B111" s="18"/>
+      <c r="C111" s="18" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="B112" s="18" t="s">
+      <c r="B112" s="18"/>
+      <c r="C112" s="18" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="B113" s="18" t="s">
+      <c r="B113" s="18"/>
+      <c r="C113" s="18" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="B114" s="18" t="s">
+      <c r="B114" s="18"/>
+      <c r="C114" s="18" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="B115" s="18" t="s">
+      <c r="B115" s="18"/>
+      <c r="C115" s="18" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="18" t="s">
         <v>336</v>
       </c>
-      <c r="B116" s="18" t="s">
+      <c r="B116" s="18"/>
+      <c r="C116" s="18" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="18" t="s">
         <v>327</v>
       </c>
-      <c r="B117" s="18" t="s">
+      <c r="B117" s="18"/>
+      <c r="C117" s="18" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="18" t="s">
         <v>329</v>
       </c>
-      <c r="B118" s="18" t="s">
+      <c r="B118" s="18"/>
+      <c r="C118" s="18" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="18" t="s">
         <v>331</v>
       </c>
-      <c r="B119" s="18" t="s">
+      <c r="B119" s="18"/>
+      <c r="C119" s="18" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="18" t="s">
         <v>333</v>
       </c>
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="18"/>
+      <c r="C120" s="18" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="B121" s="9" t="s">
+      <c r="B121" s="9"/>
+      <c r="C121" s="9" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B123" s="13" t="s">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="13" t="s">
         <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B89">
-    <sortState ref="A2:B107">
+  <autoFilter ref="A1:C89">
+    <sortState ref="A2:C107">
       <sortCondition ref="A1:A107"/>
     </sortState>
   </autoFilter>
-  <sortState ref="D2:D93">
-    <sortCondition ref="D53:D144"/>
+  <sortState ref="E2:E93">
+    <sortCondition ref="E53:E144"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -4763,13 +4952,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="225.6640625" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="225.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>227</v>
       </c>
@@ -4777,7 +4966,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>228</v>
       </c>
@@ -4785,7 +4974,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="18" t="s">
         <v>229</v>
       </c>
@@ -4793,7 +4982,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>230</v>
       </c>
@@ -4801,7 +4990,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
         <v>243</v>
       </c>
@@ -4809,7 +4998,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>231</v>
       </c>
@@ -4817,7 +5006,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>245</v>
       </c>
@@ -4825,7 +5014,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>232</v>
       </c>
@@ -4833,7 +5022,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>233</v>
       </c>
@@ -4841,7 +5030,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>234</v>
       </c>
@@ -4849,11 +5038,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>

</xml_diff>